<commit_message>
added line breaks in the descriptions so each fit in one cell
</commit_message>
<xml_diff>
--- a/swe-iday-13/idaycompanies13.xlsx
+++ b/swe-iday-13/idaycompanies13.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-20" yWindow="-20" windowWidth="21600" windowHeight="14220"/>
+    <workbookView xWindow="0" yWindow="-440" windowWidth="28720" windowHeight="17560"/>
   </bookViews>
   <sheets>
     <sheet name="smaller columns plus websites" sheetId="4" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1961" uniqueCount="270">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1924" uniqueCount="303">
   <si>
     <t>Institute for Defense Analysis</t>
   </si>
@@ -950,6 +950,142 @@
   </si>
   <si>
     <t>Careers website (opt)</t>
+  </si>
+  <si>
+    <t>Helping people make the most of their energy
+Have you ever dreamed of improving your bottom line while consuming less energy and without a power outage? We can help you solve this problem with solutions to make energy safe, reliable, efficient, productive and green from plant to plug.
+Beyond business solutions, we cover all the aspects of sustainable development: society, governance and environment. And because you cannot manage what you cannot measure, we follow our improvements with a unique tool: the Planet &amp; Society barometer.</t>
+  </si>
+  <si>
+    <t>Commonwealth Edison Company, perhaps better known as ComEd, is a unit of Chicago-based Exelon Corporation. Exelon is one of the nation's largest electric utilities, with approximately 5.4 million customers. ComEd provides service to approximately 3.8 million customers across Northern Illinois, or 70 percent of the state's population.
+ComEd is an energy delivery company. We do not own power plants and we do not make electricity. We deliver electricity to your home or business. To do this, we manage more than 90,000 miles of powerlines in an 11,400-square-mile territory. Since 2001, we have invested more than $5 billion in our electrical transmission and distributions system to continue to provide customers like you with the quality service you expect and deserve.</t>
+  </si>
+  <si>
+    <t>We are conscientious people who help others around the world fulfill their dreams of mobility. This also comprises the transport of persons, materials and information. We are aware that mobility and transport are fundamental to life, and want to help meet the high expectations in this regard.
+As a responsible, leading company and the partner of choice, we invent, develop, produce and market indispensable technological solutions that shape in particular the four mega trends, including safety, environment, information and affordable cars.</t>
+  </si>
+  <si>
+    <t>Our mission is to promote openness, innovation &amp; opportunity on the Web.
+At Mozilla, we’re a global community of technologists, thinkers and builders working together to keep the Internet alive and accessible, so people worldwide can be informed contributors and creators of the Web. We believe this act of human collaboration across an open platform is essential to individual growth and our collective future.</t>
+  </si>
+  <si>
+    <t>Whether you’re eyeing markets in the next town or across continents, we understand the importance of knowing what consumers watch and buy. That’s our passion and the very heart of our business.
+We study consumers in more than 100 countries to give you the most complete view of trends and habits worldwide. And we’re constantly evolving, not only in terms of where we measure, or what we measure, but also in how our insights can help you drive profitable growth.</t>
+  </si>
+  <si>
+    <t>Northrop Grumman is a leading global security company providing innovative systems, products and solutions in unmanned systems, cyber, C4ISR, and logistics and modernization to government and commercial customers worldwide. 
+Our mission is to be at the forefront of technology and innovation, delivering superior capability in tandem with maximized cost efficiencies. The security solutions we provide help secure freedoms for our nation as well as those of our allies. Squarely meeting our obligations, fiscally and technologically, isn't just a business goal, but a moral imperative. To that end, as we evolve as a company, the responsibility we feel for our country and the citizens and troops we help support grows with us. ​</t>
+  </si>
+  <si>
+    <t>DENSO is a global automotive supplier of advanced automotive technology, systems and components, heading toward an automotive society where cars put less drag on the environment and drivers have fewer worries about traffic accidents.
+DENSO's lead in developing this automotive society comes from anticipating the needs of automakers and closely partnering with customers right from the start.
+Our teams work quickly and diligently to manufacture products that show a commitment to safety and the environment, while at the same time punch up the level of driving comfort and convenience.</t>
+  </si>
+  <si>
+    <t>FactSet consolidates all the tools you need to monitor global markets, public and private companies, and equity and fixed income portfolios in a single, intuitive interface.
+With FactSet, you gain powerful analytics tailored to your workflow, the broadest scope of data available, and access to industry-leading client service. Our solutions are designed to fit seamlessly into your workflow, with a wide selection of customizable reports and charts that are relevant to your job function</t>
+  </si>
+  <si>
+    <t>Clarity is a data and analytics firm providing expert consulting solutions and ongoing support with an uncompromising focus on client success. Our clients trust us to produce innovative, value-driven solutions that leverage existing investments to quickly generate results. Our elite team of passionate professionals works with clients in a variety of industries throughout North America, transforming the way businesses think about, organize and use their data.
+We offer the enterprise-level expertise of a systems integrator, the client-centric focus of a boutique data services provider, and the strategic business experience of a top-tier management consulting firm. Our two subsidiaries extend and augment those offerings. Clarity Resource Group provides expert staffing solutions whether they are short-term or contract-to-hire. Clarity Operations provides a full-suite of managed services offering ensuring our clients have ongoing support for their data and analytics solutions.</t>
+  </si>
+  <si>
+    <t>Visited by more than 11 million car shoppers each month, Cars.com is the leading destination for online car shoppers, offering credible and easy-to-understand information from consumers and experts to help buyers formulate opinions on what to buy, where to buy and how much to pay for a car.
+With comprehensive pricing information, dealer reviews, side-by-side comparison tools, photo galleries, videos, unbiased editorial content and a large selection of new- and used-car inventory, Cars.com puts car buyers in control of their shopping process with the information they need to make confident buying decisions.</t>
+  </si>
+  <si>
+    <t>Illinois River Energy, LLC (IRE), owned by GTL Resources USA, Inc., operates a dry mill, corn-based bio-refinery which produces fuel grade ethanol, wet and dry distiller’s grains (ddgs), and Inedible corn oil that is utilized in the production of biodiesel and the animal feed market. The plant is located in Rochelle, Illinois where it processes over 40 million bushels of corn each year. The facility annually produces over 120 million gallons of denatured fuel grade renewable ethanol, over 300,000 tons of distiller’s grains and over 24 million pounds of Inedible corn oil.
+IRE is located on an 81 acre industrial site, southeast of Rochelle, IL at 1900 Steward Road. The facility has a positive economic impact within Rochelle and the surrounding communities. Corn is secured locally direct from farmers and through various elevators in the region.</t>
+  </si>
+  <si>
+    <t>HFZ is a firm of innovative legal professionals with several decades of combined real-world technical expertise and legal experience, proudly specializing in a broad spectrum of technical areas. We provide expert, high-value patent prosecution and counseling services to numerous companies including top patent-earning entities in the U.S.
+With actual, practical expertise in mechanical, electrical, and software arts, we craft useful claims and identify effective enforcement and defensive opportunities for your intellectual property. Throughout prosecution, HFZ keeps your business goals in mind and provides you with information you need to make business decisions.</t>
+  </si>
+  <si>
+    <t>Nokia’s mission is simple: Connecting People. Our goal is to build great mobile products that enable billions of people worldwide to enjoy more of what life has to offer. Our challenge is to achieve this in an increasingly dynamic and competitive environment.
+Ideas. Energy. Excitement. Opportunities. In today's mobile world, it feels like anything is possible - and that's what inspires us to get out of bed every day.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Goodyear Tire &amp; Rubber Company was founded in 1898 by 38-year-old Frank Seiberling.
+Looking back, the founding of The Goodyear Tire &amp; Rubber Company in 1898 seems especially remarkable, for the beginning was anything but auspicious. The 38-year-old founder, Frank A. Seiberling, purchased the company’s first plant with a $3,500 down payment -- using money he borrowed from a brother-in-law Lucius C. Miles. The rubber and cotton that were the lifeblood of the industry had to be transported from halfway around the world, to a landlocked town that had only limited rail transportation. </t>
+  </si>
+  <si>
+    <t>Hospira is the world's leading provider of injectable drugs and infusion technologies. Through our broad, integrated portfolio, we are uniquely positioned to Advance Wellness™ by improving patient and caregiver safety while reducing healthcare costs. 
+Through our offering of high-quality, lower-cost generic medications, we continue to help reduce the overall costs of healthcare — to improve both the affordability of care for patients and the financial strength of the global healthcare system.
+By working with our device customers to integrate technologies at the point of care, we are the partner of choice for improving patient and caregiver safety, clinical outcomes, cost management, as well as caregiver efficiency and effectiveness.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Over 50 years of experience has taken us across the globe from Australia to Asia, Europe and the Americas. We employ more than 18,000 people around the world and manage an extensive portfolio of assets. We’re proud to say that over a million people around the world live, work, shop or are connected through an asset we have created, every single day.  
+Our clients, partners and investors can choose to leverage our strengths and local expertise at any stage of the property and infrastructure spectrum – from development, investment management, project management &amp; construction, and asset &amp; property management – or partner with us right through the complete journey. </t>
+  </si>
+  <si>
+    <t>At McDonnell Boehnen Hulbert &amp; Berghoff LLP ("MBHB"), we provide creative, pragmatic business solutions through a variety of intellectual property services, including litigation, prosecution, and general client counseling.
+MBHB’s practice areas encompass all aspects of intellectual property law. We have practical experience in a myriad of technology areas. Our attorneys are experienced in the procurement, licensing, enforcement, and defense of patents, trademarks, copyrights, trade secrets, and unfair competition actions in a number of technological disciplines and product categories including biotechnology, business methods, chemical, electrical, mechanical and materials, pharmaceuticals and diagnostics, software and telecommunications.</t>
+  </si>
+  <si>
+    <t>Excellence. It is the foundation of everything we do. What began in 1884 with two hardworking brothers has grown into a Fortune 500 construction, mining and engineering powerhouse.
+Kiewit’s ethical, forward-thinking workforce continues to build upon the company’s reputation of safe, high-quality engineering. As an employee-owned company, Kiewit’s assets are managed by the people who know our work best. For us, business is personal. As our own stakeholders, we are invested in every project we take on. We continuously strive to build high-quality work at the lowest cost.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IMC financial markets is one of the world’s leading proprietary trading firms and a key market maker in various products listed on exchanges throughout the world.
+In general, our main strategies can be grouped into: Market Making or liquidity providing,  Algorithmic arbitrage,  Statistical arbitrage
+All of our strategies are proprietary and within IMC financial markets we do not have any external clients. All of our strategies have a short-term focus and are considered as ‘high frequency trading’. </t>
+  </si>
+  <si>
+    <t>Founded in 1984, PEC is now headquartered in Leuven, Belgium with R&amp;D and project management groups in Belgium, Hungary, the United States, China and Japan.
+Our company is staffed with highly educated experts in different technological and functional domains : Robotics, Material Handling, Power Electronics, Embedded Controls, Software , Development (.Net - Oracle), IT Security. This multidisciplinary skill matrix forms the core of PEC’s technological leadership, and creates substantial competitive advantages for our customers, in terms of quality, reliability and operational cost.</t>
+  </si>
+  <si>
+    <t>When you choose Tata Consultancy Services (TCS) as your IT services, consulting and business solutions partner, you will discover what so many global enterprises have already discovered—the power of certainty.
+We are a leader in the global marketplace and among the top 10 technology firms in the world. Our continued rapid growth is a testament to the certainty our clients experience every day. Building on more than 40 years of experience, we add real value to global organizations through domain expertise plus solutions with proven success in the field and world-class service. It’s how we keep you moving forward.</t>
+  </si>
+  <si>
+    <t>WMS is a leading global innovator in the design, manufacture and distribution of electronic and digital gaming entertainment and gaming machines for the casino industry. The WMS core values of Passion, Integrity, Innovation, Quality and Respect create a deeply embedded Culture of Innovation that fuels the imagination and creativity of our development teams and drives innovation with a purpose.
+Energized by a fervent focus on our Player Driven Innovation™ approach to product development, we create imaginative and engaging game content enabled by advanced, groundbreaking technologies to deliver dynamic, transformative player entertainment experiences in the casino and online. The talented WMS team produces some of the world's most popular casino games, and creates new and differentiated gaming platforms that consistently set the industry standard.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">United Conveyor Corporation (UCC) is a global leader in ash handling solutions for the power generation industry and a preferred supplier for dry sorbent injection and reagent handling.
+Since 1920, UCC has pioneered material handling technology and has led the way in helping to improve plant performance. UCC has devoted its efforts exclusively to the design, supply, installation and maintenance of ash handling and other abrasive material handling systems. </t>
+  </si>
+  <si>
+    <t>A community of passionate individuals whose purpose is to revolutionize software design, creation and delivery, while advocating for positive social change.
+Wherever we are in the world, ThoughtWorkers share the same cultural characteristics and imperatives. We come to work as ourselves. We enjoy each other’s company. We value honesty and transparency. Appearances and backgrounds aren’t important to us; ideas and doing the right thing are. We abhor and reject discrimination and inequality and promote diversity in all its forms. We proudly, passionately and actively strive to make both ThoughtWorks and our industry more reflective and inclusive of the society that we serve.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">We distribute our software and solutions to end users through more than 100 firms, including 19 of the top 20 U.S. futures brokers. We're proud to have the world's premier investment banks, brokers, Futures Commission Merchants (FCMs), hedge funds, proprietary trading firms and other trading institutions as our customers.
+Our customers tell us they trust TT to help them succeed in the often turbulent world of trading because of our technology, our people and our ongoing drive to innovate. We can anticipate and deliver the innovations that traders need in large part because we are intimately familiar with what they do. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">United is the world’s leading airline and is focused on being the airline customers want to fly, the airline employees want to work for and the airline shareholders want to invest in.
+United Airlines and United Express operate an average of 5,341 flights a day to more than 360 airports across six continents. In 2012, United and United Express carried more passenger traffic than any other airline in the world and operated nearly two million flights carrying 140 million customers. </t>
+  </si>
+  <si>
+    <t>Companies like P&amp;G are a force in the world. Our market capitalization is greater than the GDP of many countries, and we market our products in more than 180 countries. With this stature comes both responsibility and opportunity. Our responsibility is to be an ethical corporate citizen—but our opportunity is something far greater, and is embodied in our Purpose.
+We will provide branded products and services of superior quality and value that improve the lives of the world’s consumers, now and for generations to come. As a result, consumers will reward us with leadership sales, profit and value creation, allowing our people, our shareholders and the communities in which we live and work to prosper.</t>
+  </si>
+  <si>
+    <t>Yahoo is the world's largest start-up, which means that we move fast and always let our users lead the way. Founded in 1994 by two Stanford PhD candidates, we've grown into a company that helps you find what you're looking for on any Internet-connected device. Our employees are rewarded for curiosity and we celebrate explorers, relying on our passionate and transformative talent to do what's right for our users.
+As a leader in global daily habits like email, entertainment, news and sports, we strive to inspire, delight and entertain. By infusing our products with beauty and personality driven by our users, every Yahoo experience feels made to order.</t>
+  </si>
+  <si>
+    <t>A global leader respected for innovation and reliability, Zebra provides enabling technologies that allow customers to take smarter actions.
+Zebra's extensive portfolio of barcode, receipt, kiosk and RFID printers and supplies, as well as real-time location solutions give a digital voice to assets, people and transactions that provides greater visibility into mission-critical information.</t>
+  </si>
+  <si>
+    <t>ZS Associates is one of the world's largest business services firms specializing in transforming sales and marketing from an art to a science. We help clients gain market share at lower cost. We do so by creating data-driven strategies that they can implement rapidly and by taking on sales and marketing operations to make them more competitive. 
+With 20 offices around the world, we have worked with more than 700 companies in 70 countries across consumer products, energy, high-tech, insurance, medical products and services, pharmaceuticals and other industries.</t>
+  </si>
+  <si>
+    <t>AT&amp;T is bringing it all together for our customers, from revolutionary smartphones to next-generation TV services and sophisticated solutions for multi-national businesses.
+ For more than a century, we have consistently provided innovative, reliable, high-quality products and services and excellent customer care. Today, our mission is to connect people with their world, everywhere they live and work, and do it better than anyone else. We're fulfilling this vision by creating new solutions for consumers and businesses and by driving innovation in the communications and entertainment industry.</t>
+  </si>
+  <si>
+    <t>Imagine the power of 180,000 people with a common purpose — building relationships that create value for you and your business. This is PwC. Every day, our people work with you to build the value you are looking for.
+We bring a global perspective along with in-depth knowledge of local, state and US issues. In 1998, Price Waterhouse and Coopers &amp; Lybrand merged to create PricewaterhouseCoopers. We have a long history of delivering value-added professional services to our clients. Our accounting practice originated in London during the mid-1800's.</t>
+  </si>
+  <si>
+    <t>Readyforce was founded on the belief that the traditional job search process is broken. This is true for both job seekers and hiring companies. We exist to make the job search process better and easier.
+Finding a job is hard, lonely, time-consuming, stressful, painful...it just plain sucks. We believe that Readyforce can dramatically improve the experience by utilizing innovative technologies including social and professional networks, advance matching algorithms and web video. Readyforce will be a launching pad for people to navigate these difficult waters.</t>
   </si>
 </sst>
 </file>
@@ -1693,7 +1829,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="192">
+  <cellStyleXfs count="234">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1886,8 +2022,50 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="158">
+  <cellXfs count="175">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -2346,8 +2524,59 @@
     <xf numFmtId="0" fontId="22" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="192">
+  <cellStyles count="234">
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
@@ -2443,6 +2672,27 @@
     <cellStyle name="Followed Hyperlink" xfId="187" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="189" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="191" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="193" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="195" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="197" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="199" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="201" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="203" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="205" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="207" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="209" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="211" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="213" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="215" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="217" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="219" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="221" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="223" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="225" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="227" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="229" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="231" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="233" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
@@ -2538,6 +2788,27 @@
     <cellStyle name="Hyperlink" xfId="186" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="188" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="190" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="192" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="194" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="196" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="198" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="200" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="202" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="204" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="206" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="208" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="210" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="212" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="214" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="216" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="218" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="220" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="222" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="224" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="226" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="228" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="230" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="232" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal_Sheet1" xfId="1"/>
   </cellStyles>
@@ -2838,10 +3109,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AD86"/>
+  <dimension ref="A1:AD108"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="AB8" sqref="AB8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -2868,7 +3139,7 @@
     <col min="21" max="21" width="5.5" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="6.1640625" bestFit="1" customWidth="1"/>
     <col min="23" max="24" width="3.83203125" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="33.83203125" customWidth="1"/>
+    <col min="25" max="25" width="88.1640625" style="159" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:30" ht="44" thickTop="1" thickBot="1">
@@ -2945,7 +3216,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="2" spans="1:30" ht="16" thickTop="1">
+    <row r="2" spans="1:30" ht="76" thickTop="1">
       <c r="A2" s="133" t="s">
         <v>241</v>
       </c>
@@ -3000,11 +3271,11 @@
       <c r="X2" s="26" t="s">
         <v>111</v>
       </c>
-      <c r="Y2" s="133" t="s">
+      <c r="Y2" s="160" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="3" spans="1:30" ht="15">
+    <row r="3" spans="1:30" ht="60">
       <c r="A3" s="133" t="s">
         <v>242</v>
       </c>
@@ -3069,11 +3340,11 @@
       <c r="X3" s="33" t="s">
         <v>111</v>
       </c>
-      <c r="Y3" s="133" t="s">
+      <c r="Y3" s="160" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="4" spans="1:30" ht="15">
+    <row r="4" spans="1:30" ht="30">
       <c r="A4" s="133" t="s">
         <v>243</v>
       </c>
@@ -3124,11 +3395,11 @@
       <c r="X4" s="33" t="s">
         <v>111</v>
       </c>
-      <c r="Y4" s="133" t="s">
+      <c r="Y4" s="160" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="5" spans="1:30" ht="15">
+    <row r="5" spans="1:30" ht="75">
       <c r="A5" s="133" t="s">
         <v>244</v>
       </c>
@@ -3179,11 +3450,11 @@
       <c r="X5" s="40" t="s">
         <v>111</v>
       </c>
-      <c r="Y5" s="133" t="s">
+      <c r="Y5" s="160" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="6" spans="1:30" ht="15">
+    <row r="6" spans="1:30" ht="90">
       <c r="A6" s="133" t="s">
         <v>245</v>
       </c>
@@ -3230,11 +3501,11 @@
       <c r="X6" s="48" t="s">
         <v>111</v>
       </c>
-      <c r="Y6" s="133" t="s">
+      <c r="Y6" s="160" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="7" spans="1:30" ht="15">
+    <row r="7" spans="1:30" ht="60">
       <c r="A7" s="133"/>
       <c r="B7" s="133"/>
       <c r="C7" s="1" t="s">
@@ -3289,11 +3560,11 @@
       <c r="X7" s="50" t="s">
         <v>111</v>
       </c>
-      <c r="Y7" s="133" t="s">
+      <c r="Y7" s="160" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="8" spans="1:30" ht="15">
+    <row r="8" spans="1:30" ht="75">
       <c r="A8" s="133"/>
       <c r="B8" s="133"/>
       <c r="C8" s="2" t="s">
@@ -3334,11 +3605,11 @@
       <c r="X8" s="54" t="s">
         <v>111</v>
       </c>
-      <c r="Y8" s="133" t="s">
+      <c r="Y8" s="160" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="9" spans="1:30" ht="15">
+    <row r="9" spans="1:30" ht="105">
       <c r="C9" s="1" t="s">
         <v>14</v>
       </c>
@@ -3385,14 +3656,11 @@
       <c r="X9" s="40" t="s">
         <v>111</v>
       </c>
-      <c r="Y9" s="137" t="s">
-        <v>130</v>
-      </c>
-      <c r="Z9" s="137" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="10" spans="1:30" ht="15">
+      <c r="Y9" s="163" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="10" spans="1:30" ht="45">
       <c r="A10" s="133"/>
       <c r="B10" s="133"/>
       <c r="C10" s="1" t="s">
@@ -3435,12 +3703,12 @@
       </c>
       <c r="W10" s="29"/>
       <c r="X10" s="33"/>
-      <c r="Y10" s="133" t="s">
+      <c r="Y10" s="160" t="s">
         <v>129</v>
       </c>
       <c r="AD10" s="133"/>
     </row>
-    <row r="11" spans="1:30" ht="15">
+    <row r="11" spans="1:30" ht="75">
       <c r="A11" s="133"/>
       <c r="B11" s="133"/>
       <c r="C11" s="1" t="s">
@@ -3491,12 +3759,12 @@
       <c r="X11" s="48" t="s">
         <v>111</v>
       </c>
-      <c r="Y11" s="133" t="s">
+      <c r="Y11" s="160" t="s">
         <v>132</v>
       </c>
       <c r="AD11" s="133"/>
     </row>
-    <row r="12" spans="1:30" ht="15">
+    <row r="12" spans="1:30" ht="75">
       <c r="A12" s="133"/>
       <c r="B12" s="133"/>
       <c r="C12" s="1" t="s">
@@ -3545,12 +3813,12 @@
         <v>111</v>
       </c>
       <c r="X12" s="40"/>
-      <c r="Y12" s="133" t="s">
+      <c r="Y12" s="160" t="s">
         <v>133</v>
       </c>
       <c r="AD12" s="133"/>
     </row>
-    <row r="13" spans="1:30" ht="15">
+    <row r="13" spans="1:30" ht="105">
       <c r="A13" s="133"/>
       <c r="B13" s="133"/>
       <c r="C13" s="1" t="s">
@@ -3609,12 +3877,12 @@
       <c r="X13" s="40" t="s">
         <v>111</v>
       </c>
-      <c r="Y13" s="133" t="s">
+      <c r="Y13" s="160" t="s">
         <v>134</v>
       </c>
       <c r="AD13" s="133"/>
     </row>
-    <row r="14" spans="1:30" ht="15">
+    <row r="14" spans="1:30" ht="120">
       <c r="C14" s="1" t="s">
         <v>19</v>
       </c>
@@ -3653,14 +3921,11 @@
       <c r="X14" s="33" t="s">
         <v>111</v>
       </c>
-      <c r="Y14" s="137" t="s">
-        <v>177</v>
-      </c>
-      <c r="Z14" s="137" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="15" spans="1:30" ht="15">
+      <c r="Y14" s="163" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="15" spans="1:30" ht="45">
       <c r="A15" s="133"/>
       <c r="B15" s="133"/>
       <c r="C15" s="1" t="s">
@@ -3707,12 +3972,12 @@
       </c>
       <c r="W15" s="29"/>
       <c r="X15" s="33"/>
-      <c r="Y15" s="133" t="s">
+      <c r="Y15" s="160" t="s">
         <v>135</v>
       </c>
       <c r="AD15" s="133"/>
     </row>
-    <row r="16" spans="1:30" ht="15">
+    <row r="16" spans="1:30" ht="75">
       <c r="A16" s="134"/>
       <c r="B16" s="134"/>
       <c r="C16" s="1" t="s">
@@ -3759,12 +4024,12 @@
       <c r="X16" s="48" t="s">
         <v>111</v>
       </c>
-      <c r="Y16" s="134" t="s">
+      <c r="Y16" s="161" t="s">
         <v>136</v>
       </c>
       <c r="AD16" s="134"/>
     </row>
-    <row r="17" spans="1:30" ht="15">
+    <row r="17" spans="1:30" ht="60">
       <c r="A17" s="133"/>
       <c r="B17" s="133"/>
       <c r="C17" s="1" t="s">
@@ -3813,12 +4078,12 @@
       <c r="X17" s="40" t="s">
         <v>111</v>
       </c>
-      <c r="Y17" s="133" t="s">
+      <c r="Y17" s="160" t="s">
         <v>137</v>
       </c>
       <c r="AD17" s="133"/>
     </row>
-    <row r="18" spans="1:30" ht="15">
+    <row r="18" spans="1:30" ht="165">
       <c r="C18" s="1" t="s">
         <v>23</v>
       </c>
@@ -3867,14 +4132,11 @@
       </c>
       <c r="W18" s="52"/>
       <c r="X18" s="40"/>
-      <c r="Y18" s="137" t="s">
-        <v>179</v>
-      </c>
-      <c r="Z18" s="137" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="19" spans="1:30" ht="15">
+      <c r="Y18" s="163" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="19" spans="1:30" ht="60">
       <c r="A19" s="133"/>
       <c r="B19" s="133"/>
       <c r="C19" s="1" t="s">
@@ -3915,12 +4177,12 @@
       </c>
       <c r="W19" s="34"/>
       <c r="X19" s="40"/>
-      <c r="Y19" s="133" t="s">
+      <c r="Y19" s="160" t="s">
         <v>138</v>
       </c>
       <c r="AD19" s="133"/>
     </row>
-    <row r="20" spans="1:30" ht="15">
+    <row r="20" spans="1:30" ht="150">
       <c r="C20" s="1" t="s">
         <v>25</v>
       </c>
@@ -3961,11 +4223,8 @@
       <c r="X20" s="65" t="s">
         <v>111</v>
       </c>
-      <c r="Y20" s="138" t="s">
-        <v>181</v>
-      </c>
-      <c r="Z20" s="138" t="s">
-        <v>182</v>
+      <c r="Y20" s="162" t="s">
+        <v>271</v>
       </c>
     </row>
     <row r="21" spans="1:30">
@@ -3982,7 +4241,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="22" spans="1:30" ht="15">
+    <row r="22" spans="1:30" ht="105">
       <c r="C22" s="1" t="s">
         <v>26</v>
       </c>
@@ -4027,14 +4286,11 @@
       <c r="X22" s="72" t="s">
         <v>111</v>
       </c>
-      <c r="Y22" s="137" t="s">
-        <v>183</v>
-      </c>
-      <c r="Z22" s="137" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="23" spans="1:30" ht="15">
+      <c r="Y22" s="163" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="23" spans="1:30" ht="60">
       <c r="A23" s="133" t="s">
         <v>246</v>
       </c>
@@ -4097,11 +4353,11 @@
       </c>
       <c r="W23" s="35"/>
       <c r="X23" s="36"/>
-      <c r="Y23" s="133" t="s">
+      <c r="Y23" s="160" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="24" spans="1:30" ht="15">
+    <row r="24" spans="1:30" ht="135">
       <c r="A24" t="s">
         <v>247</v>
       </c>
@@ -4153,17 +4409,11 @@
       <c r="X24" s="33" t="s">
         <v>111</v>
       </c>
-      <c r="Y24" s="139" t="s">
-        <v>172</v>
-      </c>
-      <c r="Z24" s="139" t="s">
-        <v>173</v>
-      </c>
-      <c r="AA24" s="139" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="25" spans="1:30" ht="15">
+      <c r="Y24" s="164" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="25" spans="1:30" ht="90">
       <c r="A25" s="133" t="s">
         <v>251</v>
       </c>
@@ -4206,11 +4456,11 @@
       </c>
       <c r="W25" s="29"/>
       <c r="X25" s="33"/>
-      <c r="Y25" s="133" t="s">
+      <c r="Y25" s="160" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="26" spans="1:30" ht="15">
+    <row r="26" spans="1:30" ht="45">
       <c r="A26" s="133" t="s">
         <v>250</v>
       </c>
@@ -4257,11 +4507,11 @@
       </c>
       <c r="W26" s="77"/>
       <c r="X26" s="79"/>
-      <c r="Y26" s="133" t="s">
+      <c r="Y26" s="160" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="27" spans="1:30" ht="15">
+    <row r="27" spans="1:30" ht="75">
       <c r="A27" s="133"/>
       <c r="B27" s="133"/>
       <c r="C27" s="1" t="s">
@@ -4324,11 +4574,11 @@
       </c>
       <c r="W27" s="29"/>
       <c r="X27" s="40"/>
-      <c r="Y27" s="133" t="s">
+      <c r="Y27" s="160" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="28" spans="1:30" ht="15">
+    <row r="28" spans="1:30" ht="90">
       <c r="A28" s="133" t="s">
         <v>248</v>
       </c>
@@ -4375,11 +4625,11 @@
       <c r="X28" s="40" t="s">
         <v>111</v>
       </c>
-      <c r="Y28" s="133" t="s">
+      <c r="Y28" s="160" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="29" spans="1:30" ht="15">
+    <row r="29" spans="1:30" ht="60">
       <c r="A29" s="133"/>
       <c r="B29" s="133"/>
       <c r="C29" s="1" t="s">
@@ -4442,11 +4692,11 @@
       </c>
       <c r="W29" s="34"/>
       <c r="X29" s="33"/>
-      <c r="Y29" s="133" t="s">
+      <c r="Y29" s="160" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="30" spans="1:30" ht="15">
+    <row r="30" spans="1:30" ht="105">
       <c r="A30" s="133"/>
       <c r="B30" s="133"/>
       <c r="C30" s="1" t="s">
@@ -4491,11 +4741,11 @@
       <c r="X30" s="40" t="s">
         <v>111</v>
       </c>
-      <c r="Y30" s="133" t="s">
+      <c r="Y30" s="160" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="31" spans="1:30" ht="15">
+    <row r="31" spans="1:30" ht="75">
       <c r="A31" s="133"/>
       <c r="B31" s="133"/>
       <c r="C31" s="1" t="s">
@@ -4550,11 +4800,11 @@
       <c r="X31" s="40" t="s">
         <v>111</v>
       </c>
-      <c r="Y31" s="133" t="s">
+      <c r="Y31" s="160" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="32" spans="1:30" ht="15">
+    <row r="32" spans="1:30" ht="45">
       <c r="A32" s="133"/>
       <c r="B32" s="133"/>
       <c r="C32" s="1" t="s">
@@ -4595,11 +4845,11 @@
       <c r="X32" s="40" t="s">
         <v>111</v>
       </c>
-      <c r="Y32" s="133" t="s">
+      <c r="Y32" s="160" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="33" spans="1:27" ht="15">
+    <row r="33" spans="1:25" ht="90">
       <c r="A33" t="s">
         <v>249</v>
       </c>
@@ -4645,14 +4895,11 @@
       <c r="X33" s="33" t="s">
         <v>111</v>
       </c>
-      <c r="Y33" s="139" t="s">
-        <v>175</v>
-      </c>
-      <c r="Z33" s="139" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="34" spans="1:27" ht="15">
+      <c r="Y33" s="164" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="34" spans="1:25" ht="45">
       <c r="A34" s="133" t="s">
         <v>253</v>
       </c>
@@ -4703,11 +4950,11 @@
       <c r="X34" s="40" t="s">
         <v>111</v>
       </c>
-      <c r="Y34" s="133" t="s">
+      <c r="Y34" s="160" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="35" spans="1:27" ht="15">
+    <row r="35" spans="1:25" ht="90">
       <c r="A35" s="133"/>
       <c r="B35" s="133"/>
       <c r="C35" s="1" t="s">
@@ -4758,11 +5005,11 @@
       <c r="X35" s="33" t="s">
         <v>111</v>
       </c>
-      <c r="Y35" s="133" t="s">
+      <c r="Y35" s="160" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="36" spans="1:27" ht="15">
+    <row r="36" spans="1:25" ht="60">
       <c r="A36" s="133" t="s">
         <v>252</v>
       </c>
@@ -4803,11 +5050,11 @@
       <c r="X36" s="40" t="s">
         <v>111</v>
       </c>
-      <c r="Y36" s="133" t="s">
+      <c r="Y36" s="160" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="37" spans="1:27" ht="16" thickBot="1">
+    <row r="37" spans="1:25" ht="61" thickBot="1">
       <c r="A37" s="133"/>
       <c r="B37" s="133"/>
       <c r="C37" s="1" t="s">
@@ -4852,11 +5099,11 @@
         <v>111</v>
       </c>
       <c r="X37" s="33"/>
-      <c r="Y37" s="133" t="s">
+      <c r="Y37" s="160" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="38" spans="1:27" ht="17" thickTop="1" thickBot="1">
+    <row r="38" spans="1:25" ht="92" thickTop="1" thickBot="1">
       <c r="A38" s="133" t="s">
         <v>255</v>
       </c>
@@ -4909,11 +5156,11 @@
       </c>
       <c r="W38" s="84"/>
       <c r="X38" s="88"/>
-      <c r="Y38" s="133" t="s">
+      <c r="Y38" s="160" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="39" spans="1:27" ht="16" thickTop="1">
+    <row r="39" spans="1:25" ht="76" thickTop="1">
       <c r="A39" s="133"/>
       <c r="B39" s="133"/>
       <c r="C39" s="1" t="s">
@@ -4982,11 +5229,11 @@
       <c r="X39" s="40" t="s">
         <v>111</v>
       </c>
-      <c r="Y39" s="133" t="s">
+      <c r="Y39" s="160" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="40" spans="1:27" ht="15">
+    <row r="40" spans="1:25" ht="105">
       <c r="C40" s="1" t="s">
         <v>42</v>
       </c>
@@ -5033,14 +5280,11 @@
       <c r="X40" s="40" t="s">
         <v>111</v>
       </c>
-      <c r="Y40" s="139" t="s">
-        <v>185</v>
-      </c>
-      <c r="Z40" s="139" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="41" spans="1:27" ht="15">
+      <c r="Y40" s="164" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="41" spans="1:25" ht="150">
       <c r="C41" s="1" t="s">
         <v>43</v>
       </c>
@@ -5079,14 +5323,11 @@
       <c r="X41" s="95" t="s">
         <v>111</v>
       </c>
-      <c r="Y41" s="137" t="s">
-        <v>187</v>
-      </c>
-      <c r="Z41" s="137" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="42" spans="1:27" ht="15">
+      <c r="Y41" s="163" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="42" spans="1:25" ht="135">
       <c r="A42" t="s">
         <v>254</v>
       </c>
@@ -5132,14 +5373,11 @@
       </c>
       <c r="W42" s="29"/>
       <c r="X42" s="33"/>
-      <c r="Y42" s="133" t="s">
-        <v>189</v>
-      </c>
-      <c r="Z42" s="133" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="43" spans="1:27" ht="15">
+      <c r="Y42" s="163" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="43" spans="1:25" ht="90">
       <c r="A43" t="s">
         <v>258</v>
       </c>
@@ -5188,14 +5426,11 @@
       <c r="X43" s="40" t="s">
         <v>111</v>
       </c>
-      <c r="Y43" s="139" t="s">
-        <v>191</v>
-      </c>
-      <c r="Z43" s="139" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="44" spans="1:27" ht="15">
+      <c r="Y43" s="164" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="44" spans="1:25" ht="165">
       <c r="A44" t="s">
         <v>257</v>
       </c>
@@ -5249,17 +5484,11 @@
         <v>111</v>
       </c>
       <c r="X44" s="33"/>
-      <c r="Y44" s="137" t="s">
-        <v>193</v>
-      </c>
-      <c r="Z44" s="137" t="s">
-        <v>194</v>
-      </c>
-      <c r="AA44" s="137" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="45" spans="1:27" ht="15">
+      <c r="Y44" s="163" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="45" spans="1:25" ht="75">
       <c r="A45" s="135"/>
       <c r="B45" s="135"/>
       <c r="C45" s="1" t="s">
@@ -5298,11 +5527,11 @@
       </c>
       <c r="W45" s="29"/>
       <c r="X45" s="33"/>
-      <c r="Y45" s="135" t="s">
+      <c r="Y45" s="165" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="46" spans="1:27" ht="15">
+    <row r="46" spans="1:25" ht="120">
       <c r="C46" s="1" t="s">
         <v>48</v>
       </c>
@@ -5347,17 +5576,11 @@
       <c r="X46" s="40" t="s">
         <v>111</v>
       </c>
-      <c r="Y46" s="139" t="s">
-        <v>196</v>
-      </c>
-      <c r="Z46" s="139" t="s">
-        <v>197</v>
-      </c>
-      <c r="AA46" s="139" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="47" spans="1:27">
+      <c r="Y46" s="164" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="47" spans="1:25">
       <c r="C47" s="156" t="s">
         <v>0</v>
       </c>
@@ -5413,7 +5636,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="48" spans="1:27" ht="15">
+    <row r="48" spans="1:25" ht="60">
       <c r="A48" s="133"/>
       <c r="B48" s="133"/>
       <c r="C48" s="1" t="s">
@@ -5464,11 +5687,11 @@
       <c r="X48" s="95" t="s">
         <v>111</v>
       </c>
-      <c r="Y48" s="133" t="s">
+      <c r="Y48" s="160" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="49" spans="1:26" ht="15">
+    <row r="49" spans="1:26" ht="105">
       <c r="C49" s="1" t="s">
         <v>5</v>
       </c>
@@ -5511,14 +5734,12 @@
       <c r="X49" s="95" t="s">
         <v>111</v>
       </c>
-      <c r="Y49" s="133" t="s">
-        <v>199</v>
-      </c>
-      <c r="Z49" s="133" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="50" spans="1:26" ht="15">
+      <c r="Y49" s="160" t="s">
+        <v>287</v>
+      </c>
+      <c r="Z49" s="133"/>
+    </row>
+    <row r="50" spans="1:26" ht="120">
       <c r="C50" s="1" t="s">
         <v>87</v>
       </c>
@@ -5557,14 +5778,11 @@
       <c r="X50" s="95" t="s">
         <v>111</v>
       </c>
-      <c r="Y50" s="139" t="s">
-        <v>201</v>
-      </c>
-      <c r="Z50" s="139" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="51" spans="1:26" ht="15">
+      <c r="Y50" s="164" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="51" spans="1:26" ht="30">
       <c r="A51" s="133"/>
       <c r="B51" s="133"/>
       <c r="C51" s="1" t="s">
@@ -5615,11 +5833,11 @@
       <c r="X51" s="65" t="s">
         <v>111</v>
       </c>
-      <c r="Y51" s="133" t="s">
+      <c r="Y51" s="160" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="52" spans="1:26" ht="15">
+    <row r="52" spans="1:26" ht="135">
       <c r="C52" s="1" t="s">
         <v>50</v>
       </c>
@@ -5664,14 +5882,11 @@
       </c>
       <c r="W52" s="99"/>
       <c r="X52" s="100"/>
-      <c r="Y52" s="141" t="s">
-        <v>203</v>
-      </c>
-      <c r="Z52" s="141" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="53" spans="1:26" ht="15">
+      <c r="Y52" s="166" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="53" spans="1:26" ht="105">
       <c r="A53" s="136"/>
       <c r="B53" s="136"/>
       <c r="C53" s="1" t="s">
@@ -5718,11 +5933,11 @@
       </c>
       <c r="W53" s="99"/>
       <c r="X53" s="100"/>
-      <c r="Y53" s="136" t="s">
+      <c r="Y53" s="167" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="54" spans="1:26" ht="28">
+    <row r="54" spans="1:26" ht="75">
       <c r="A54" s="133"/>
       <c r="B54" s="133"/>
       <c r="C54" s="3" t="s">
@@ -5767,11 +5982,11 @@
       </c>
       <c r="W54" s="61"/>
       <c r="X54" s="95"/>
-      <c r="Y54" s="133" t="s">
+      <c r="Y54" s="160" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="55" spans="1:26" ht="15">
+    <row r="55" spans="1:26" ht="90">
       <c r="A55" s="133"/>
       <c r="B55" s="133"/>
       <c r="C55" s="1" t="s">
@@ -5820,11 +6035,11 @@
       <c r="X55" s="48" t="s">
         <v>111</v>
       </c>
-      <c r="Y55" s="133" t="s">
+      <c r="Y55" s="160" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="56" spans="1:26" ht="15">
+    <row r="56" spans="1:26" ht="90">
       <c r="C56" s="1" t="s">
         <v>54</v>
       </c>
@@ -5861,14 +6076,12 @@
       <c r="X56" s="108" t="s">
         <v>111</v>
       </c>
-      <c r="Y56" s="133" t="s">
-        <v>205</v>
-      </c>
-      <c r="Z56" s="133" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="57" spans="1:26" ht="15">
+      <c r="Y56" s="160" t="s">
+        <v>273</v>
+      </c>
+      <c r="Z56" s="133"/>
+    </row>
+    <row r="57" spans="1:26" ht="90">
       <c r="C57" s="1" t="s">
         <v>55</v>
       </c>
@@ -5929,14 +6142,11 @@
       <c r="X57" s="115" t="s">
         <v>111</v>
       </c>
-      <c r="Y57" s="142" t="s">
-        <v>207</v>
-      </c>
-      <c r="Z57" s="142" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="58" spans="1:26" ht="15">
+      <c r="Y57" s="168" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="58" spans="1:26" ht="135">
       <c r="C58" s="1" t="s">
         <v>56</v>
       </c>
@@ -5979,14 +6189,11 @@
       <c r="X58" s="108" t="s">
         <v>111</v>
       </c>
-      <c r="Y58" s="143" t="s">
-        <v>209</v>
-      </c>
-      <c r="Z58" s="143" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="59" spans="1:26" ht="15">
+      <c r="Y58" s="169" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="59" spans="1:26" ht="75">
       <c r="A59" s="133"/>
       <c r="B59" s="133"/>
       <c r="C59" s="1" t="s">
@@ -6029,11 +6236,11 @@
       <c r="X59" s="40" t="s">
         <v>111</v>
       </c>
-      <c r="Y59" s="133" t="s">
+      <c r="Y59" s="160" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="60" spans="1:26" ht="15">
+    <row r="60" spans="1:26" ht="60">
       <c r="A60" s="133"/>
       <c r="B60" s="133"/>
       <c r="C60" s="2" t="s">
@@ -6096,11 +6303,11 @@
       </c>
       <c r="W60" s="34"/>
       <c r="X60" s="40"/>
-      <c r="Y60" s="133" t="s">
+      <c r="Y60" s="160" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="61" spans="1:26" ht="15">
+    <row r="61" spans="1:26" ht="75">
       <c r="A61" s="133"/>
       <c r="B61" s="133"/>
       <c r="C61" s="1" t="s">
@@ -6141,11 +6348,11 @@
       </c>
       <c r="W61" s="34"/>
       <c r="X61" s="33"/>
-      <c r="Y61" s="133" t="s">
+      <c r="Y61" s="160" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="62" spans="1:26" ht="15">
+    <row r="62" spans="1:26" ht="135">
       <c r="C62" s="1" t="s">
         <v>60</v>
       </c>
@@ -6196,14 +6403,11 @@
       <c r="X62" s="50" t="s">
         <v>111</v>
       </c>
-      <c r="Y62" s="137" t="s">
-        <v>211</v>
-      </c>
-      <c r="Z62" s="137" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="63" spans="1:26" ht="15">
+      <c r="Y62" s="163" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="63" spans="1:26" ht="75">
       <c r="A63" s="133"/>
       <c r="B63" s="133"/>
       <c r="C63" s="1" t="s">
@@ -6246,11 +6450,11 @@
       </c>
       <c r="W63" s="44"/>
       <c r="X63" s="50"/>
-      <c r="Y63" s="133" t="s">
+      <c r="Y63" s="160" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="64" spans="1:26" ht="15">
+    <row r="64" spans="1:26" ht="120">
       <c r="C64" s="1" t="s">
         <v>62</v>
       </c>
@@ -6291,14 +6495,11 @@
       </c>
       <c r="W64" s="29"/>
       <c r="X64" s="33"/>
-      <c r="Y64" s="137" t="s">
-        <v>213</v>
-      </c>
-      <c r="Z64" s="137" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="65" spans="1:27" ht="15">
+      <c r="Y64" s="163" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="65" spans="1:25" ht="135">
       <c r="A65" s="133"/>
       <c r="B65" s="133"/>
       <c r="C65" s="1" t="s">
@@ -6341,11 +6542,11 @@
       <c r="V65" s="32"/>
       <c r="W65" s="29"/>
       <c r="X65" s="33"/>
-      <c r="Y65" s="133" t="s">
+      <c r="Y65" s="160" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="66" spans="1:27" ht="15">
+    <row r="66" spans="1:25" ht="90">
       <c r="A66" s="133"/>
       <c r="B66" s="133"/>
       <c r="C66" s="1" t="s">
@@ -6388,11 +6589,11 @@
       </c>
       <c r="W66" s="29"/>
       <c r="X66" s="33"/>
-      <c r="Y66" s="133" t="s">
+      <c r="Y66" s="160" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="67" spans="1:27" ht="15">
+    <row r="67" spans="1:25" ht="120">
       <c r="C67" s="1" t="s">
         <v>65</v>
       </c>
@@ -6449,14 +6650,11 @@
       <c r="X67" s="33" t="s">
         <v>111</v>
       </c>
-      <c r="Y67" s="144" t="s">
-        <v>215</v>
-      </c>
-      <c r="Z67" s="144" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="68" spans="1:27" ht="15">
+      <c r="Y67" s="158" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="68" spans="1:25" ht="105">
       <c r="C68" s="1" t="s">
         <v>66</v>
       </c>
@@ -6507,14 +6705,11 @@
       <c r="X68" s="33" t="s">
         <v>111</v>
       </c>
-      <c r="Y68" s="145" t="s">
-        <v>217</v>
-      </c>
-      <c r="Z68" s="145" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="69" spans="1:27">
+      <c r="Y68" s="170" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="69" spans="1:25">
       <c r="C69" s="156" t="s">
         <v>1</v>
       </c>
@@ -6529,7 +6724,7 @@
       </c>
       <c r="G69" s="132"/>
     </row>
-    <row r="70" spans="1:27" ht="16" thickBot="1">
+    <row r="70" spans="1:25" ht="76" thickBot="1">
       <c r="A70" s="133"/>
       <c r="B70" s="133"/>
       <c r="C70" s="1" t="s">
@@ -6574,11 +6769,11 @@
       </c>
       <c r="W70" s="34"/>
       <c r="X70" s="33"/>
-      <c r="Y70" s="133" t="s">
+      <c r="Y70" s="160" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="71" spans="1:27" ht="17" thickTop="1" thickBot="1">
+    <row r="71" spans="1:25" ht="122" thickTop="1" thickBot="1">
       <c r="A71" s="133"/>
       <c r="B71" s="133"/>
       <c r="C71" s="1" t="s">
@@ -6625,11 +6820,11 @@
       <c r="X71" s="121" t="s">
         <v>111</v>
       </c>
-      <c r="Y71" s="133" t="s">
+      <c r="Y71" s="160" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="72" spans="1:27" ht="15">
+    <row r="72" spans="1:25" ht="135">
       <c r="A72" t="s">
         <v>267</v>
       </c>
@@ -6685,17 +6880,11 @@
       <c r="X72" s="40" t="s">
         <v>111</v>
       </c>
-      <c r="Y72" s="144" t="s">
-        <v>220</v>
-      </c>
-      <c r="Z72" s="144" t="s">
-        <v>221</v>
-      </c>
-      <c r="AA72" s="144" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="73" spans="1:27" ht="15">
+      <c r="Y72" s="158" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="73" spans="1:25" ht="60">
       <c r="A73" s="133"/>
       <c r="B73" s="133"/>
       <c r="C73" s="1" t="s">
@@ -6742,11 +6931,11 @@
       <c r="X73" s="33" t="s">
         <v>111</v>
       </c>
-      <c r="Y73" s="133" t="s">
+      <c r="Y73" s="160" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="74" spans="1:27" ht="15">
+    <row r="74" spans="1:25" ht="90">
       <c r="A74" s="133" t="s">
         <v>260</v>
       </c>
@@ -6805,11 +6994,11 @@
       <c r="X74" s="50" t="s">
         <v>111</v>
       </c>
-      <c r="Y74" s="133" t="s">
+      <c r="Y74" s="160" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="75" spans="1:27" ht="15">
+    <row r="75" spans="1:25" ht="105">
       <c r="A75" t="s">
         <v>262</v>
       </c>
@@ -6855,14 +7044,11 @@
       </c>
       <c r="W75" s="34"/>
       <c r="X75" s="33"/>
-      <c r="Y75" s="137" t="s">
-        <v>223</v>
-      </c>
-      <c r="Z75" s="137" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="76" spans="1:27" ht="15">
+      <c r="Y75" s="163" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="76" spans="1:25" ht="60">
       <c r="A76" s="133" t="s">
         <v>261</v>
       </c>
@@ -6905,11 +7091,11 @@
       <c r="X76" s="40" t="s">
         <v>111</v>
       </c>
-      <c r="Y76" s="133" t="s">
+      <c r="Y76" s="160" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="77" spans="1:27" ht="15">
+    <row r="77" spans="1:25" ht="135">
       <c r="C77" s="1" t="s">
         <v>74</v>
       </c>
@@ -6970,14 +7156,11 @@
       </c>
       <c r="W77" s="34"/>
       <c r="X77" s="33"/>
-      <c r="Y77" s="146" t="s">
-        <v>225</v>
-      </c>
-      <c r="Z77" s="146" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="78" spans="1:27" ht="15">
+      <c r="Y77" s="171" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="78" spans="1:25" ht="120">
       <c r="C78" s="1" t="s">
         <v>75</v>
       </c>
@@ -7018,14 +7201,11 @@
       <c r="X78" s="40" t="s">
         <v>111</v>
       </c>
-      <c r="Y78" s="147" t="s">
-        <v>227</v>
-      </c>
-      <c r="Z78" s="147" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="79" spans="1:27" ht="15">
+      <c r="Y78" s="172" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="79" spans="1:25" ht="90">
       <c r="C79" s="4" t="s">
         <v>76</v>
       </c>
@@ -7068,14 +7248,11 @@
       <c r="X79" s="40" t="s">
         <v>111</v>
       </c>
-      <c r="Y79" s="133" t="s">
-        <v>229</v>
-      </c>
-      <c r="Z79" s="133" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="80" spans="1:27" ht="15">
+      <c r="Y79" s="160" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="80" spans="1:25" ht="90">
       <c r="C80" s="1" t="s">
         <v>77</v>
       </c>
@@ -7116,14 +7293,11 @@
       </c>
       <c r="W80" s="29"/>
       <c r="X80" s="33"/>
-      <c r="Y80" s="147" t="s">
-        <v>231</v>
-      </c>
-      <c r="Z80" s="147" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="81" spans="1:26" ht="15">
+      <c r="Y80" s="172" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="81" spans="1:25" ht="90">
       <c r="A81" s="133"/>
       <c r="B81" s="133"/>
       <c r="C81" s="1" t="s">
@@ -7162,11 +7336,11 @@
         <v>111</v>
       </c>
       <c r="X81" s="48"/>
-      <c r="Y81" s="133" t="s">
+      <c r="Y81" s="160" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="82" spans="1:26" ht="15">
+    <row r="82" spans="1:25" ht="150">
       <c r="C82" s="4" t="s">
         <v>79</v>
       </c>
@@ -7219,14 +7393,11 @@
       <c r="X82" s="40" t="s">
         <v>111</v>
       </c>
-      <c r="Y82" s="137" t="s">
-        <v>239</v>
-      </c>
-      <c r="Z82" s="137" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="83" spans="1:26" ht="15">
+      <c r="Y82" s="163" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="83" spans="1:25" ht="75">
       <c r="A83" s="133" t="s">
         <v>263</v>
       </c>
@@ -7273,11 +7444,11 @@
       <c r="X83" s="33" t="s">
         <v>111</v>
       </c>
-      <c r="Y83" s="133" t="s">
+      <c r="Y83" s="160" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="84" spans="1:26" ht="15">
+    <row r="84" spans="1:25" ht="120">
       <c r="C84" s="1" t="s">
         <v>81</v>
       </c>
@@ -7320,14 +7491,11 @@
       <c r="X84" s="95" t="s">
         <v>111</v>
       </c>
-      <c r="Y84" s="149" t="s">
-        <v>237</v>
-      </c>
-      <c r="Z84" s="149" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="85" spans="1:26" ht="15">
+      <c r="Y84" s="173" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="85" spans="1:25" ht="90">
       <c r="A85" t="s">
         <v>264</v>
       </c>
@@ -7381,14 +7549,11 @@
       <c r="X85" s="40" t="s">
         <v>111</v>
       </c>
-      <c r="Y85" s="148" t="s">
-        <v>235</v>
-      </c>
-      <c r="Z85" s="148" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="86" spans="1:26" ht="15">
+      <c r="Y85" s="174" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="86" spans="1:25" ht="120">
       <c r="A86" t="s">
         <v>265</v>
       </c>
@@ -7457,12 +7622,12 @@
       <c r="X86" s="129" t="s">
         <v>111</v>
       </c>
-      <c r="Y86" s="147" t="s">
-        <v>233</v>
-      </c>
-      <c r="Z86" s="147" t="s">
-        <v>234</v>
-      </c>
+      <c r="Y86" s="172" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="108" spans="25:25">
+      <c r="Y108"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
add abbreviations of majors
</commit_message>
<xml_diff>
--- a/swe-iday-13/idaycompanies13.xlsx
+++ b/swe-iday-13/idaycompanies13.xlsx
@@ -4,13 +4,13 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="-440" windowWidth="28720" windowHeight="17560"/>
+    <workbookView xWindow="7140" yWindow="0" windowWidth="28720" windowHeight="17560" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="smaller columns plus websites" sheetId="4" r:id="rId1"/>
     <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId3"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId4"/>
+    <sheet name="major abbreviations" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1924" uniqueCount="303">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1984" uniqueCount="342">
   <si>
     <t>Institute for Defense Analysis</t>
   </si>
@@ -1087,12 +1087,129 @@
     <t>Readyforce was founded on the belief that the traditional job search process is broken. This is true for both job seekers and hiring companies. We exist to make the job search process better and easier.
 Finding a job is hard, lonely, time-consuming, stressful, painful...it just plain sucks. We believe that Readyforce can dramatically improve the experience by utilizing innovative technologies including social and professional networks, advance matching algorithms and web video. Readyforce will be a launching pad for people to navigate these difficult waters.</t>
   </si>
+  <si>
+    <t>http://www.mccormick.northwestern.edu/mcd/Students/Events/techexpo.html</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Abbreviations according to </t>
+  </si>
+  <si>
+    <t>Co-op = Walter P. Murphy Cooperative Engineering Education Program - minimum of 4 quarter commitment</t>
+  </si>
+  <si>
+    <t>AM = Applied Mathematics</t>
+  </si>
+  <si>
+    <t>BME = Biomedical Engineering</t>
+  </si>
+  <si>
+    <t>CHE = Chemical Engineering</t>
+  </si>
+  <si>
+    <t>CE = Civil Engineering</t>
+  </si>
+  <si>
+    <t>CMPE = Computer Engineering</t>
+  </si>
+  <si>
+    <t>CS = Computer Science</t>
+  </si>
+  <si>
+    <t>EE = Electrical Engineering</t>
+  </si>
+  <si>
+    <t>EnvE = Environmental Engineering</t>
+  </si>
+  <si>
+    <t>FT = Full Time Employment</t>
+  </si>
+  <si>
+    <t>IE = Industrial Engineering</t>
+  </si>
+  <si>
+    <t>MBP = Masters of Biotechnology Program</t>
+  </si>
+  <si>
+    <t>MaDE = Manufacturing and Design Engineering</t>
+  </si>
+  <si>
+    <t>MEM = Masters of Engineering Management</t>
+  </si>
+  <si>
+    <t>MPM = Masters of Product Management</t>
+  </si>
+  <si>
+    <t>MSE = Materials Science and Engineering</t>
+  </si>
+  <si>
+    <t>MSEDI = Masters of Science Engineering Design and Innovation</t>
+  </si>
+  <si>
+    <t>MSITP = Masters of Science Information Technology Program</t>
+  </si>
+  <si>
+    <t>ME = Mechanical Engineering</t>
+  </si>
+  <si>
+    <t>SL = Service Learning Project</t>
+  </si>
+  <si>
+    <t>TAM = Theoretical and Applied Math</t>
+  </si>
+  <si>
+    <t>AM</t>
+  </si>
+  <si>
+    <t>CHE</t>
+  </si>
+  <si>
+    <t>CE</t>
+  </si>
+  <si>
+    <t>CMPE</t>
+  </si>
+  <si>
+    <t>CS</t>
+  </si>
+  <si>
+    <t>EnvE</t>
+  </si>
+  <si>
+    <t>FT</t>
+  </si>
+  <si>
+    <t>MBP</t>
+  </si>
+  <si>
+    <t>MEM</t>
+  </si>
+  <si>
+    <t>MPM</t>
+  </si>
+  <si>
+    <t>MSE</t>
+  </si>
+  <si>
+    <t>MSEDI</t>
+  </si>
+  <si>
+    <t>MSITP</t>
+  </si>
+  <si>
+    <t>ME</t>
+  </si>
+  <si>
+    <t>SL</t>
+  </si>
+  <si>
+    <t>TAM</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="23" x14ac:knownFonts="1">
+  <fonts count="24" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1224,6 +1341,11 @@
     <font>
       <sz val="10"/>
       <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
   </fonts>
@@ -1829,7 +1951,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="234">
+  <cellStyleXfs count="286">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -2064,8 +2186,60 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="175">
+  <cellXfs count="178">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -2575,8 +2749,11 @@
     <xf numFmtId="0" fontId="13" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="234">
+  <cellStyles count="286">
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
@@ -2693,6 +2870,32 @@
     <cellStyle name="Followed Hyperlink" xfId="229" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="231" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="233" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="235" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="237" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="239" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="241" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="243" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="245" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="247" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="249" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="251" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="253" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="255" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="257" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="259" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="261" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="263" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="265" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="267" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="269" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="271" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="273" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="275" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="277" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="279" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="281" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="283" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="285" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
@@ -2809,6 +3012,32 @@
     <cellStyle name="Hyperlink" xfId="228" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="230" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="232" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="234" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="236" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="238" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="240" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="242" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="244" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="246" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="248" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="250" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="252" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="254" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="256" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="258" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="260" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="262" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="264" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="266" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="268" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="270" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="272" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="274" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="276" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="278" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="280" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="282" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="284" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal_Sheet1" xfId="1"/>
   </cellStyles>
@@ -3109,10 +3338,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AD108"/>
+  <dimension ref="A1:Z108"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="AB8" sqref="AB8"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="X1" sqref="H1:X1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -3140,9 +3369,11 @@
     <col min="22" max="22" width="6.1640625" bestFit="1" customWidth="1"/>
     <col min="23" max="24" width="3.83203125" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="88.1640625" style="159" customWidth="1"/>
+    <col min="29" max="29" width="55.33203125" customWidth="1"/>
+    <col min="30" max="30" width="8.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" ht="44" thickTop="1" thickBot="1">
+    <row r="1" spans="1:25" ht="44" thickTop="1" thickBot="1">
       <c r="A1" t="s">
         <v>268</v>
       </c>
@@ -3216,7 +3447,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="2" spans="1:30" ht="76" thickTop="1">
+    <row r="2" spans="1:25" ht="76" thickTop="1">
       <c r="A2" s="133" t="s">
         <v>241</v>
       </c>
@@ -3275,7 +3506,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="3" spans="1:30" ht="60">
+    <row r="3" spans="1:25" ht="60">
       <c r="A3" s="133" t="s">
         <v>242</v>
       </c>
@@ -3344,7 +3575,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="4" spans="1:30" ht="30">
+    <row r="4" spans="1:25" ht="30">
       <c r="A4" s="133" t="s">
         <v>243</v>
       </c>
@@ -3399,7 +3630,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="5" spans="1:30" ht="75">
+    <row r="5" spans="1:25" ht="75">
       <c r="A5" s="133" t="s">
         <v>244</v>
       </c>
@@ -3454,7 +3685,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="6" spans="1:30" ht="90">
+    <row r="6" spans="1:25" ht="90">
       <c r="A6" s="133" t="s">
         <v>245</v>
       </c>
@@ -3505,7 +3736,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="7" spans="1:30" ht="60">
+    <row r="7" spans="1:25" ht="60">
       <c r="A7" s="133"/>
       <c r="B7" s="133"/>
       <c r="C7" s="1" t="s">
@@ -3564,7 +3795,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="8" spans="1:30" ht="75">
+    <row r="8" spans="1:25" ht="75">
       <c r="A8" s="133"/>
       <c r="B8" s="133"/>
       <c r="C8" s="2" t="s">
@@ -3609,7 +3840,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="9" spans="1:30" ht="105">
+    <row r="9" spans="1:25" ht="105">
       <c r="C9" s="1" t="s">
         <v>14</v>
       </c>
@@ -3660,7 +3891,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="10" spans="1:30" ht="45">
+    <row r="10" spans="1:25" ht="45">
       <c r="A10" s="133"/>
       <c r="B10" s="133"/>
       <c r="C10" s="1" t="s">
@@ -3706,9 +3937,8 @@
       <c r="Y10" s="160" t="s">
         <v>129</v>
       </c>
-      <c r="AD10" s="133"/>
-    </row>
-    <row r="11" spans="1:30" ht="75">
+    </row>
+    <row r="11" spans="1:25" ht="75">
       <c r="A11" s="133"/>
       <c r="B11" s="133"/>
       <c r="C11" s="1" t="s">
@@ -3762,9 +3992,8 @@
       <c r="Y11" s="160" t="s">
         <v>132</v>
       </c>
-      <c r="AD11" s="133"/>
-    </row>
-    <row r="12" spans="1:30" ht="75">
+    </row>
+    <row r="12" spans="1:25" ht="75">
       <c r="A12" s="133"/>
       <c r="B12" s="133"/>
       <c r="C12" s="1" t="s">
@@ -3816,9 +4045,8 @@
       <c r="Y12" s="160" t="s">
         <v>133</v>
       </c>
-      <c r="AD12" s="133"/>
-    </row>
-    <row r="13" spans="1:30" ht="105">
+    </row>
+    <row r="13" spans="1:25" ht="105">
       <c r="A13" s="133"/>
       <c r="B13" s="133"/>
       <c r="C13" s="1" t="s">
@@ -3880,9 +4108,8 @@
       <c r="Y13" s="160" t="s">
         <v>134</v>
       </c>
-      <c r="AD13" s="133"/>
-    </row>
-    <row r="14" spans="1:30" ht="120">
+    </row>
+    <row r="14" spans="1:25" ht="120">
       <c r="C14" s="1" t="s">
         <v>19</v>
       </c>
@@ -3925,7 +4152,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="15" spans="1:30" ht="45">
+    <row r="15" spans="1:25" ht="45">
       <c r="A15" s="133"/>
       <c r="B15" s="133"/>
       <c r="C15" s="1" t="s">
@@ -3975,9 +4202,8 @@
       <c r="Y15" s="160" t="s">
         <v>135</v>
       </c>
-      <c r="AD15" s="133"/>
-    </row>
-    <row r="16" spans="1:30" ht="75">
+    </row>
+    <row r="16" spans="1:25" ht="75">
       <c r="A16" s="134"/>
       <c r="B16" s="134"/>
       <c r="C16" s="1" t="s">
@@ -4027,9 +4253,8 @@
       <c r="Y16" s="161" t="s">
         <v>136</v>
       </c>
-      <c r="AD16" s="134"/>
-    </row>
-    <row r="17" spans="1:30" ht="60">
+    </row>
+    <row r="17" spans="1:25" ht="60">
       <c r="A17" s="133"/>
       <c r="B17" s="133"/>
       <c r="C17" s="1" t="s">
@@ -4081,9 +4306,8 @@
       <c r="Y17" s="160" t="s">
         <v>137</v>
       </c>
-      <c r="AD17" s="133"/>
-    </row>
-    <row r="18" spans="1:30" ht="165">
+    </row>
+    <row r="18" spans="1:25" ht="165">
       <c r="C18" s="1" t="s">
         <v>23</v>
       </c>
@@ -4136,7 +4360,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="19" spans="1:30" ht="60">
+    <row r="19" spans="1:25" ht="60">
       <c r="A19" s="133"/>
       <c r="B19" s="133"/>
       <c r="C19" s="1" t="s">
@@ -4180,9 +4404,8 @@
       <c r="Y19" s="160" t="s">
         <v>138</v>
       </c>
-      <c r="AD19" s="133"/>
-    </row>
-    <row r="20" spans="1:30" ht="150">
+    </row>
+    <row r="20" spans="1:25" ht="150">
       <c r="C20" s="1" t="s">
         <v>25</v>
       </c>
@@ -4227,7 +4450,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="21" spans="1:30">
+    <row r="21" spans="1:25">
       <c r="C21" s="5" t="s">
         <v>6</v>
       </c>
@@ -4241,7 +4464,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="22" spans="1:30" ht="105">
+    <row r="22" spans="1:25" ht="105">
       <c r="C22" s="1" t="s">
         <v>26</v>
       </c>
@@ -4290,7 +4513,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="23" spans="1:30" ht="60">
+    <row r="23" spans="1:25" ht="60">
       <c r="A23" s="133" t="s">
         <v>246</v>
       </c>
@@ -4357,7 +4580,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="24" spans="1:30" ht="135">
+    <row r="24" spans="1:25" ht="135">
       <c r="A24" t="s">
         <v>247</v>
       </c>
@@ -4413,7 +4636,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="25" spans="1:30" ht="90">
+    <row r="25" spans="1:25" ht="90">
       <c r="A25" s="133" t="s">
         <v>251</v>
       </c>
@@ -4460,7 +4683,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="26" spans="1:30" ht="45">
+    <row r="26" spans="1:25" ht="45">
       <c r="A26" s="133" t="s">
         <v>250</v>
       </c>
@@ -4511,7 +4734,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="27" spans="1:30" ht="75">
+    <row r="27" spans="1:25" ht="75">
       <c r="A27" s="133"/>
       <c r="B27" s="133"/>
       <c r="C27" s="1" t="s">
@@ -4578,7 +4801,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="28" spans="1:30" ht="90">
+    <row r="28" spans="1:25" ht="90">
       <c r="A28" s="133" t="s">
         <v>248</v>
       </c>
@@ -4629,7 +4852,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="29" spans="1:30" ht="60">
+    <row r="29" spans="1:25" ht="60">
       <c r="A29" s="133"/>
       <c r="B29" s="133"/>
       <c r="C29" s="1" t="s">
@@ -4696,7 +4919,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="30" spans="1:30" ht="105">
+    <row r="30" spans="1:25" ht="105">
       <c r="A30" s="133"/>
       <c r="B30" s="133"/>
       <c r="C30" s="1" t="s">
@@ -4745,7 +4968,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="31" spans="1:30" ht="75">
+    <row r="31" spans="1:25" ht="75">
       <c r="A31" s="133"/>
       <c r="B31" s="133"/>
       <c r="C31" s="1" t="s">
@@ -4804,7 +5027,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="32" spans="1:30" ht="45">
+    <row r="32" spans="1:25" ht="45">
       <c r="A32" s="133"/>
       <c r="B32" s="133"/>
       <c r="C32" s="1" t="s">
@@ -12109,12 +12332,345 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:E44"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A21" sqref="A21"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="54.1640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" t="s">
+        <v>304</v>
+      </c>
+      <c r="D1" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="175" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" s="176" t="s">
+        <v>306</v>
+      </c>
+      <c r="B3" s="176" t="s">
+        <v>326</v>
+      </c>
+      <c r="C3" s="176"/>
+      <c r="D3" s="176"/>
+      <c r="E3" s="176"/>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" s="176" t="s">
+        <v>307</v>
+      </c>
+      <c r="B4" s="176" t="s">
+        <v>95</v>
+      </c>
+      <c r="C4" s="176"/>
+      <c r="D4" s="176"/>
+      <c r="E4" s="176"/>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" s="176" t="s">
+        <v>308</v>
+      </c>
+      <c r="B5" s="176" t="s">
+        <v>327</v>
+      </c>
+      <c r="C5" s="176"/>
+      <c r="D5" s="176"/>
+      <c r="E5" s="176"/>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" s="176" t="s">
+        <v>309</v>
+      </c>
+      <c r="B6" s="176" t="s">
+        <v>328</v>
+      </c>
+      <c r="C6" s="176"/>
+      <c r="D6" s="176"/>
+      <c r="E6" s="176"/>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" s="176" t="s">
+        <v>310</v>
+      </c>
+      <c r="B7" s="176" t="s">
+        <v>329</v>
+      </c>
+      <c r="C7" s="176"/>
+      <c r="D7" s="176"/>
+      <c r="E7" s="176"/>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" s="176" t="s">
+        <v>311</v>
+      </c>
+      <c r="B8" s="176" t="s">
+        <v>330</v>
+      </c>
+      <c r="C8" s="176"/>
+      <c r="D8" s="176"/>
+      <c r="E8" s="176"/>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" s="176" t="s">
+        <v>312</v>
+      </c>
+      <c r="B9" s="176" t="s">
+        <v>100</v>
+      </c>
+      <c r="C9" s="176"/>
+      <c r="D9" s="176"/>
+      <c r="E9" s="176"/>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" s="176" t="s">
+        <v>313</v>
+      </c>
+      <c r="B10" s="176" t="s">
+        <v>331</v>
+      </c>
+      <c r="C10" s="176"/>
+      <c r="D10" s="176"/>
+      <c r="E10" s="176"/>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" s="176" t="s">
+        <v>314</v>
+      </c>
+      <c r="B11" s="176" t="s">
+        <v>332</v>
+      </c>
+      <c r="C11" s="176"/>
+      <c r="D11" s="176"/>
+      <c r="E11" s="176"/>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" s="176" t="s">
+        <v>315</v>
+      </c>
+      <c r="B12" s="176" t="s">
+        <v>102</v>
+      </c>
+      <c r="C12" s="176"/>
+      <c r="D12" s="176"/>
+      <c r="E12" s="176"/>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" s="176" t="s">
+        <v>316</v>
+      </c>
+      <c r="B13" s="176" t="s">
+        <v>333</v>
+      </c>
+      <c r="C13" s="176"/>
+      <c r="D13" s="176"/>
+      <c r="E13" s="176"/>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" s="176" t="s">
+        <v>317</v>
+      </c>
+      <c r="B14" s="176" t="s">
+        <v>103</v>
+      </c>
+      <c r="C14" s="176"/>
+      <c r="D14" s="176"/>
+      <c r="E14" s="176"/>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15" s="176" t="s">
+        <v>318</v>
+      </c>
+      <c r="B15" s="176" t="s">
+        <v>334</v>
+      </c>
+      <c r="C15" s="176"/>
+      <c r="D15" s="176"/>
+      <c r="E15" s="176"/>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16" s="176" t="s">
+        <v>319</v>
+      </c>
+      <c r="B16" s="176" t="s">
+        <v>335</v>
+      </c>
+      <c r="C16" s="176"/>
+      <c r="D16" s="176"/>
+      <c r="E16" s="176"/>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17" s="176" t="s">
+        <v>320</v>
+      </c>
+      <c r="B17" s="176" t="s">
+        <v>336</v>
+      </c>
+      <c r="C17" s="176"/>
+      <c r="D17" s="176"/>
+      <c r="E17" s="176"/>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="A18" s="176" t="s">
+        <v>321</v>
+      </c>
+      <c r="B18" s="176" t="s">
+        <v>337</v>
+      </c>
+      <c r="C18" s="176"/>
+      <c r="D18" s="176"/>
+      <c r="E18" s="176"/>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="A19" s="176" t="s">
+        <v>322</v>
+      </c>
+      <c r="B19" s="176" t="s">
+        <v>338</v>
+      </c>
+      <c r="C19" s="176"/>
+      <c r="D19" s="176"/>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="A20" t="s">
+        <v>323</v>
+      </c>
+      <c r="B20" s="177" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="A21" t="s">
+        <v>324</v>
+      </c>
+      <c r="B21" s="177" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5">
+      <c r="A22" t="s">
+        <v>325</v>
+      </c>
+      <c r="B22" s="177" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5">
+      <c r="A23" s="176"/>
+      <c r="B23" s="176"/>
+      <c r="C23" s="176"/>
+      <c r="D23" s="176"/>
+      <c r="E23" s="176"/>
+    </row>
+    <row r="24" spans="1:5">
+      <c r="A24" s="176"/>
+    </row>
+    <row r="25" spans="1:5">
+      <c r="A25" s="176"/>
+    </row>
+    <row r="26" spans="1:5">
+      <c r="A26" s="176"/>
+    </row>
+    <row r="27" spans="1:5">
+      <c r="A27" s="176" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5">
+      <c r="A28" s="176" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5">
+      <c r="A29" s="176" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5">
+      <c r="A30" s="176" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5">
+      <c r="A31" s="176" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5">
+      <c r="A32" s="176" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1">
+      <c r="A33" s="176" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1">
+      <c r="A34" s="176" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1">
+      <c r="A35" s="176" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1">
+      <c r="A36" s="176" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1">
+      <c r="A37" s="176" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1">
+      <c r="A38" s="176" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1">
+      <c r="A39" s="176" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1">
+      <c r="A40" s="176" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1">
+      <c r="A41" s="176" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1">
+      <c r="A42" s="176" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1">
+      <c r="A43" s="176" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1">
+      <c r="A44" s="176"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">

</xml_diff>